<commit_message>
Update, chia lại task, theo dõi mà làm nha mọi người. #LongDB
</commit_message>
<xml_diff>
--- a/wiki/plan/Daily Tasksheet.xlsx
+++ b/wiki/plan/Daily Tasksheet.xlsx
@@ -309,16 +309,16 @@
     <t>Coding</t>
   </si>
   <si>
-    <t>Trips, routes, stations, coaches management</t>
-  </si>
-  <si>
-    <t>Users, staffs management</t>
-  </si>
-  <si>
-    <t>Scheduling, assigning management</t>
-  </si>
-  <si>
     <t>Requests, packages, comments and rating management</t>
+  </si>
+  <si>
+    <t>Coaches, coache types, volume management</t>
+  </si>
+  <si>
+    <t>Trips, routes, stations management</t>
+  </si>
+  <si>
+    <t>Scheduling, assigning, staffs management</t>
   </si>
 </sst>
 </file>
@@ -920,8 +920,8 @@
   <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD66"/>
+      <pane ySplit="12" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2363,7 +2363,7 @@
         <v>61</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C69" s="36"/>
       <c r="D69" s="16" t="s">
@@ -2382,7 +2382,7 @@
         <v>62</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C70" s="40" t="s">
         <v>2</v>
@@ -2401,7 +2401,7 @@
         <v>63</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C71" s="40"/>
       <c r="D71" s="16"/>

</xml_diff>

<commit_message>
Update Daily Tasksheet.xlsx #LongDB
</commit_message>
<xml_diff>
--- a/wiki/plan/Daily Tasksheet.xlsx
+++ b/wiki/plan/Daily Tasksheet.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="85">
   <si>
     <t>No.</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>Admin functions: Staffs management, Fee management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online payment (bạn anh LỮ) </t>
   </si>
 </sst>
 </file>
@@ -892,7 +895,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
+      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2353,9 +2356,13 @@
       <c r="A79" s="24">
         <v>76</v>
       </c>
-      <c r="B79" s="18"/>
+      <c r="B79" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="C79" s="21"/>
-      <c r="D79" s="10"/>
+      <c r="D79" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="E79" s="21"/>
       <c r="F79" s="18"/>
       <c r="G79" s="33"/>

</xml_diff>

<commit_message>
Cập nhật Daily Tasksheet.xlsx Thêm file Notes.xlsx để ghi chú những thay đổi chưa cập nhật toàn bộ #LongDB
</commit_message>
<xml_diff>
--- a/wiki/plan/Daily Tasksheet.xlsx
+++ b/wiki/plan/Daily Tasksheet.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
   <si>
     <t>No.</t>
   </si>
@@ -895,7 +895,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
+      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2232,7 +2232,9 @@
       </c>
       <c r="F71" s="17"/>
       <c r="G71" s="33"/>
-      <c r="H71" s="25"/>
+      <c r="H71" s="25" t="s">
+        <v>2</v>
+      </c>
       <c r="I71" s="18"/>
     </row>
     <row r="72" spans="1:9" ht="15.75">
@@ -2244,7 +2246,9 @@
       </c>
       <c r="C72" s="18"/>
       <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
+      <c r="E72" s="27" t="s">
+        <v>2</v>
+      </c>
       <c r="F72" s="18"/>
       <c r="G72" s="33"/>
       <c r="H72" s="25" t="s">
@@ -2261,7 +2265,9 @@
       </c>
       <c r="C73" s="18"/>
       <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
+      <c r="E73" s="27" t="s">
+        <v>2</v>
+      </c>
       <c r="F73" s="18"/>
       <c r="G73" s="33"/>
       <c r="H73" s="25" t="s">
@@ -2278,10 +2284,14 @@
       </c>
       <c r="C74" s="18"/>
       <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
+      <c r="E74" s="27" t="s">
+        <v>2</v>
+      </c>
       <c r="F74" s="18"/>
       <c r="G74" s="33"/>
-      <c r="H74" s="25"/>
+      <c r="H74" s="25" t="s">
+        <v>2</v>
+      </c>
       <c r="I74" s="18"/>
     </row>
     <row r="75" spans="1:9" ht="15.75">
@@ -2346,7 +2356,9 @@
       </c>
       <c r="C78" s="21"/>
       <c r="D78" s="10"/>
-      <c r="E78" s="21"/>
+      <c r="E78" s="21" t="s">
+        <v>2</v>
+      </c>
       <c r="F78" s="10"/>
       <c r="G78" s="33"/>
       <c r="H78" s="25"/>
@@ -2788,7 +2800,7 @@
     <mergeCell ref="A8:A12"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F92:F93 E23:E41 C86:D93 E90:E109 D2:E22 E44:E66 F85 F90 F95:F96 F98 F100:F101 F105:F106 F103 F108 F80 C2:C67 C95:C100 D76:D85 F82:F83 F87:F88 C70:E71 E68 D23:D69 E76:E87 C76:C84 F2:F71 H2:H119 F75:F78">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F92:F93 E23:E41 C86:D93 E90:E109 D2:E22 E44:E66 F85 F90 F95:F96 F98 F100:F101 F105:F106 F103 F108 F80 C2:C67 C95:C100 D76:D85 F82:F83 F87:F88 C70:E71 E68 D23:D69 E76:E87 C76:C84 F2:F71 H2:H119 F75:F78 E72:E74">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Daily Tasksheet.xlsx ngày 24/3 #LongDB
</commit_message>
<xml_diff>
--- a/wiki/plan/Daily Tasksheet.xlsx
+++ b/wiki/plan/Daily Tasksheet.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="90">
   <si>
     <t>No.</t>
   </si>
@@ -324,9 +324,6 @@
     <t>Admin functions: Staffs management, Fee management</t>
   </si>
   <si>
-    <t xml:space="preserve">Online payment (bạn anh LỮ) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Return </t>
   </si>
   <si>
@@ -334,6 +331,21 @@
   </si>
   <si>
     <t>Manage request status (role Staff)</t>
+  </si>
+  <si>
+    <t>Trip management: manage departure &amp; arrival time</t>
+  </si>
+  <si>
+    <t>Invoice: export &amp; print</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online payment </t>
+  </si>
+  <si>
+    <t>Late payment</t>
+  </si>
+  <si>
+    <t>Assign</t>
   </si>
 </sst>
 </file>
@@ -505,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -600,11 +612,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -911,8 +934,8 @@
   <dimension ref="A1:I119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77:H77"/>
+      <pane ySplit="12" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -957,7 +980,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A2" s="36">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -974,7 +997,7 @@
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A3" s="36"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
@@ -989,7 +1012,7 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1004,7 +1027,7 @@
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1021,7 +1044,7 @@
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1057,7 @@
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
@@ -1047,7 +1070,7 @@
       <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A8" s="36">
+      <c r="A8" s="37">
         <v>2</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -1062,7 +1085,7 @@
       <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
@@ -1075,7 +1098,7 @@
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="11" t="s">
         <v>5</v>
       </c>
@@ -1088,7 +1111,7 @@
       <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
@@ -1101,7 +1124,7 @@
       <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" hidden="1" customHeight="1">
-      <c r="A12" s="36"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
@@ -2257,7 +2280,7 @@
         <v>66</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C72" s="27"/>
       <c r="D72" s="18"/>
@@ -2294,8 +2317,8 @@
       <c r="A74" s="24">
         <v>68</v>
       </c>
-      <c r="B74" s="37" t="s">
-        <v>83</v>
+      <c r="B74" s="36" t="s">
+        <v>82</v>
       </c>
       <c r="C74" s="27" t="s">
         <v>2</v>
@@ -2388,7 +2411,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="20" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C79" s="21"/>
       <c r="D79" s="10" t="s">
@@ -2407,7 +2430,7 @@
         <v>77</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C80" s="21" t="s">
         <v>2</v>
@@ -2422,24 +2445,28 @@
       <c r="I80" s="18"/>
     </row>
     <row r="81" spans="1:9" ht="15.75">
-      <c r="A81" s="24">
-        <v>78</v>
-      </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="33"/>
+      <c r="A81" s="38"/>
+      <c r="B81" s="39">
+        <v>41722</v>
+      </c>
+      <c r="C81" s="40"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="40"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="42"/>
       <c r="H81" s="25"/>
-      <c r="I81" s="18"/>
+      <c r="I81" s="41"/>
     </row>
     <row r="82" spans="1:9" ht="15.75">
       <c r="A82" s="24">
-        <v>79</v>
-      </c>
-      <c r="B82" s="18"/>
-      <c r="C82" s="21"/>
+        <v>78</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>2</v>
+      </c>
       <c r="D82" s="10"/>
       <c r="E82" s="21"/>
       <c r="F82" s="10"/>
@@ -2449,24 +2476,34 @@
     </row>
     <row r="83" spans="1:9" ht="15.75">
       <c r="A83" s="24">
-        <v>80</v>
-      </c>
-      <c r="B83" s="18"/>
+        <v>79</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>86</v>
+      </c>
       <c r="C83" s="21"/>
       <c r="D83" s="10"/>
       <c r="E83" s="21"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="33"/>
+      <c r="F83" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G83" s="33">
+        <v>41724</v>
+      </c>
       <c r="H83" s="25"/>
       <c r="I83" s="18"/>
     </row>
     <row r="84" spans="1:9" ht="15.75">
       <c r="A84" s="24">
-        <v>81</v>
-      </c>
-      <c r="B84" s="18"/>
+        <v>80</v>
+      </c>
+      <c r="B84" s="20" t="s">
+        <v>88</v>
+      </c>
       <c r="C84" s="21"/>
-      <c r="D84" s="10"/>
+      <c r="D84" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="E84" s="21"/>
       <c r="F84" s="18"/>
       <c r="G84" s="33"/>
@@ -2475,12 +2512,16 @@
     </row>
     <row r="85" spans="1:9" ht="15.75">
       <c r="A85" s="24">
-        <v>82</v>
-      </c>
-      <c r="B85" s="18"/>
+        <v>81</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="C85" s="18"/>
       <c r="D85" s="10"/>
-      <c r="E85" s="21"/>
+      <c r="E85" s="21" t="s">
+        <v>2</v>
+      </c>
       <c r="F85" s="10"/>
       <c r="G85" s="33"/>
       <c r="H85" s="25"/>
@@ -2488,7 +2529,7 @@
     </row>
     <row r="86" spans="1:9" ht="15.75">
       <c r="A86" s="24">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B86" s="18"/>
       <c r="C86" s="21"/>
@@ -2501,7 +2542,7 @@
     </row>
     <row r="87" spans="1:9" ht="15.75">
       <c r="A87" s="24">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B87" s="18"/>
       <c r="C87" s="21"/>
@@ -2514,7 +2555,7 @@
     </row>
     <row r="88" spans="1:9" ht="15.75">
       <c r="A88" s="24">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B88" s="18"/>
       <c r="C88" s="21"/>
@@ -2527,7 +2568,7 @@
     </row>
     <row r="89" spans="1:9" ht="15.75">
       <c r="A89" s="24">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B89" s="18"/>
       <c r="C89" s="21"/>
@@ -2540,7 +2581,7 @@
     </row>
     <row r="90" spans="1:9" ht="15.75">
       <c r="A90" s="24">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B90" s="18"/>
       <c r="C90" s="21"/>
@@ -2553,7 +2594,7 @@
     </row>
     <row r="91" spans="1:9" ht="15.75">
       <c r="A91" s="24">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" s="18"/>
       <c r="C91" s="21"/>
@@ -2566,7 +2607,7 @@
     </row>
     <row r="92" spans="1:9" ht="15.75">
       <c r="A92" s="24">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B92" s="18"/>
       <c r="C92" s="21"/>
@@ -2579,7 +2620,7 @@
     </row>
     <row r="93" spans="1:9" ht="15.75">
       <c r="A93" s="24">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B93" s="18"/>
       <c r="C93" s="21"/>
@@ -2592,7 +2633,7 @@
     </row>
     <row r="94" spans="1:9" ht="15.75">
       <c r="A94" s="24">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B94" s="18"/>
       <c r="C94" s="18"/>
@@ -2605,7 +2646,7 @@
     </row>
     <row r="95" spans="1:9" ht="15.75">
       <c r="A95" s="24">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B95" s="18"/>
       <c r="C95" s="10"/>
@@ -2617,7 +2658,9 @@
       <c r="I95" s="18"/>
     </row>
     <row r="96" spans="1:9" ht="15.75">
-      <c r="A96" s="6"/>
+      <c r="A96" s="24">
+        <v>92</v>
+      </c>
       <c r="B96" s="18"/>
       <c r="C96" s="10"/>
       <c r="D96" s="18"/>

</xml_diff>